<commit_message>
Final Script + Excel
</commit_message>
<xml_diff>
--- a/HexData/ExampleDataTemplate.xlsx
+++ b/HexData/ExampleDataTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Mol.E-coder\HexData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD6CD9F8-D6DA-40D8-8865-CB01641C7062}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0533CE-B9DC-49B8-96B7-238CE8C90D42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28035" yWindow="2550" windowWidth="28800" windowHeight="15435" xr2:uid="{4BCB3082-D71E-447B-A2C7-ED0A06A4C62C}"/>
+    <workbookView xWindow="4740" yWindow="1905" windowWidth="19260" windowHeight="15435" xr2:uid="{4BCB3082-D71E-447B-A2C7-ED0A06A4C62C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -294,9 +294,6 @@
     <t>1655.8, 1444.7, 1261.5, 1130.5, 987.4, 796.3, 613.2, 498.2, 319.1</t>
   </si>
   <si>
-    <t>1660.8, 1483.7, 1352.6, 1209.7, 1024.4, 831.3, 688.3, 587.2, 410.1, 265.0</t>
-  </si>
-  <si>
     <t>1700.7, 1523.6, 1344.5, 1167.5, 1066.5, 887.4, 702.3, 599.2, 470.2, 279.1</t>
   </si>
   <si>
@@ -309,9 +306,6 @@
     <t>1892.5, 1715.5, 1504.5, 1327.5, 1198.4, 985.4, 802.3, 623.2, 410.2, 279.1</t>
   </si>
   <si>
-    <t>1656.7, 1479.6, 1348.6, 1205.5, 1074.4, 929.3, 750.3, 573.2, 456.1, 327.1</t>
-  </si>
-  <si>
     <t>1686.6, 1509.6, 1364.5, 1261.5, 1146.4, 935.4, 758.3, 615.3, 472.1, 329.1</t>
   </si>
   <si>
@@ -322,6 +316,12 @@
   </si>
   <si>
     <t xml:space="preserve">1850.8, 1673.8, 1482.8, 1303.6, 1120.5, 991.4, 848.3, 657.3, 512.2, 319.1 </t>
+  </si>
+  <si>
+    <t>1660.8, 1483.7, 1340.6, 1209.7, 1024.4, 831.3, 688.3, 587.2, 410.1, 265.0</t>
+  </si>
+  <si>
+    <t>1656.7, 1479.6, 1336.6, 1205.5, 1074.4, 929.3, 750.3, 573.2, 456.1, 327.1</t>
   </si>
 </sst>
 </file>
@@ -750,7 +750,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,45 +997,45 @@
         <v>80</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>81</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>85</v>
       </c>
       <c r="I7" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="K7" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="K7" s="9" t="s">
-        <v>90</v>
-      </c>
       <c r="L7" s="9" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="150" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>84</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>95</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>82</v>

</xml_diff>